<commit_message>
updated test for footer
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Professional\Desktop\edX_UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73868F91-CD83-4AFD-B916-B9CF10E040CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2946E7E7-BA8A-469A-8AB9-700EAF4D5B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>DASHBOARD</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>Observe titles of tabs</t>
-  </si>
-  <si>
-    <t>Observe the Courses tab</t>
-  </si>
-  <si>
-    <t>The Courses tab is selected by default</t>
   </si>
   <si>
     <t>Click on EDX logo on the Global Header</t>
@@ -211,9 +205,6 @@
 -edX for Business</t>
   </si>
   <si>
-    <t>Verify that all elements are links</t>
-  </si>
-  <si>
     <t>Observe the Legal list</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
 - Discover Now</t>
   </si>
   <si>
-    <t>active state ?</t>
-  </si>
-  <si>
     <t>Click on the Discover New tab</t>
   </si>
   <si>
@@ -261,6 +249,18 @@
   </si>
   <si>
     <t>depends on test1</t>
+  </si>
+  <si>
+    <t>Verify that all elements are have the correct color and font</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedIn has a capthcha </t>
+  </si>
+  <si>
+    <t>Verify that the social media links on the page have the correct URLs</t>
+  </si>
+  <si>
+    <t>edX Facebook/Twitter/LinkedIn/Instagram/Reddit have correct links</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,10 +694,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -711,120 +711,106 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -834,10 +820,13 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -845,15 +834,21 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -861,15 +856,18 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -877,15 +875,21 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,17 +897,37 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -913,20 +937,20 @@
         <v>15</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -934,10 +958,10 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,15 +969,15 @@
         <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -961,10 +985,10 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -972,10 +996,10 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -983,10 +1007,10 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for course dashboard page
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Professional\Desktop\edX_UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2946E7E7-BA8A-469A-8AB9-700EAF4D5B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3DD37D-0EF6-4F06-84FE-06DFA6BF6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>DASHBOARD</t>
   </si>
@@ -75,9 +75,6 @@
 - Account
 - Order History
 - Sign Out</t>
-  </si>
-  <si>
-    <t>Courses</t>
   </si>
   <si>
     <r>
@@ -113,9 +110,6 @@
     <t>"Explore Courses" button is enabled</t>
   </si>
   <si>
-    <t>Click on the "Explore Courses" button</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -157,9 +151,6 @@
 - Explore New Course button</t>
   </si>
   <si>
-    <t>Click on the "Explore New Courses" button</t>
-  </si>
-  <si>
     <t>"my-courses" component is displayed
 The message "You are not enrolled in any courses yet" is not present on the Course Dashboard</t>
   </si>
@@ -229,10 +220,6 @@
     <t>The edX Home Page is present</t>
   </si>
   <si>
-    <t>The button is clickable. 
-The system redirects user to the "https://www.edx.org/search"</t>
-  </si>
-  <si>
     <t>passed</t>
   </si>
   <si>
@@ -261,6 +248,24 @@
   </si>
   <si>
     <t>edX Facebook/Twitter/LinkedIn/Instagram/Reddit have correct links</t>
+  </si>
+  <si>
+    <t>Courses Dashboard</t>
+  </si>
+  <si>
+    <t>Backgroud is black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The button is clickable. </t>
+  </si>
+  <si>
+    <t>Verify that the "Explore New Courses" button is enabled</t>
+  </si>
+  <si>
+    <t>Observe the course options. Try to delete course using the unenroll option</t>
+  </si>
+  <si>
+    <t>the course was unenrolled from course dashboard</t>
   </si>
 </sst>
 </file>
@@ -635,11 +640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,10 +699,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -711,10 +716,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -742,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,13 +755,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,13 +769,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -778,13 +783,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -792,25 +797,25 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -820,13 +825,13 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -834,21 +839,21 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -856,18 +861,18 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -875,21 +880,21 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -897,13 +902,13 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -911,106 +916,140 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="2" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
-        <v>17</v>
+      <c r="D26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>16</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>17</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="C31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C32" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>21</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>46</v>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>